<commit_message>
updated 2020/03/20 10:30am ET
</commit_message>
<xml_diff>
--- a/ON_Stat.xlsx
+++ b/ON_Stat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyq92\Documents\R\Covid19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43381DED-8BC1-4AA8-A3A1-5528ED99D6CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052E20CC-E506-408A-B45F-D00D4DD2A189}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E9AEFF62-3E62-4167-9002-420000B7859E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$258</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$R$259</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="156">
   <si>
     <t>Case number</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Hamilton Public Health</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Sunnybrook</t>
   </si>
   <si>
@@ -447,13 +444,70 @@
   </si>
   <si>
     <t>Manila</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/coronavirus-update-1.5473473</t>
+  </si>
+  <si>
+    <t>https://www.thespec.com/news-story/9866405-5th-presumptive-case-of-covid-19-in-ontario-ministry-of-health-says/</t>
+  </si>
+  <si>
+    <t>https://www.cbc.ca/news/canada/toronto/ontario-covid-19-coronavirus-iran-husband-1.5477831</t>
+  </si>
+  <si>
+    <t>https://globalnews.ca/news/6608901/toronto-coronavirus-covid-19-ontario-7th-case/</t>
+  </si>
+  <si>
+    <t>https://globalnews.ca/news/6612317/covid-19-eighth-case-ontario/</t>
+  </si>
+  <si>
+    <t>https://dailyhive.com/vancouver/ontario-4-cases-coronavirus</t>
+  </si>
+  <si>
+    <t>https://www.ctvnews.ca/health/coronavirus/tracking-every-case-of-covid-19-in-canada-1.4852102</t>
+  </si>
+  <si>
+    <t>deceased</t>
+  </si>
+  <si>
+    <t>travel (USA)</t>
+  </si>
+  <si>
+    <t>Peterborough</t>
+  </si>
+  <si>
+    <t>travel (cruise)</t>
+  </si>
+  <si>
+    <t>travel (Caribbean cruise)</t>
+  </si>
+  <si>
+    <t>Hastings Prince Edward</t>
+  </si>
+  <si>
+    <t>travel (Bahamas)</t>
+  </si>
+  <si>
+    <t>LTCH</t>
+  </si>
+  <si>
+    <t>travel (Portugal)</t>
+  </si>
+  <si>
+    <t>travel (Caribbean)</t>
+  </si>
+  <si>
+    <t>90s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,6 +519,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -487,18 +549,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -811,11 +876,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F50E69-EDCB-4C99-8A27-E7B5995F0020}">
-  <dimension ref="A1:R258"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:R309"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H266" sqref="B266:H269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -835,31 +901,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -867,31 +936,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
         <v>82</v>
-      </c>
-      <c r="C2" t="s">
-        <v>83</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" t="s">
         <v>96</v>
-      </c>
-      <c r="G2" t="s">
-        <v>97</v>
       </c>
       <c r="H2" t="s">
         <v>23</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J2" s="3">
         <v>43855</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -899,16 +971,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -917,10 +989,13 @@
         <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J3" s="3">
         <v>43857</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -928,60 +1003,66 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" t="s">
         <v>96</v>
       </c>
-      <c r="G4" t="s">
-        <v>97</v>
-      </c>
       <c r="H4" t="s">
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J4" s="3">
         <v>43861</v>
       </c>
+      <c r="L4" s="4" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" t="s">
         <v>96</v>
-      </c>
-      <c r="G5" t="s">
-        <v>97</v>
       </c>
       <c r="H5" t="s">
         <v>4</v>
       </c>
       <c r="J5" s="3">
         <v>43884</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -989,28 +1070,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H6" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="3">
         <v>43887</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
@@ -1018,10 +1102,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -1036,10 +1120,13 @@
         <v>4</v>
       </c>
       <c r="I7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J7" s="3">
         <v>43888</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -1047,28 +1134,31 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
         <v>82</v>
-      </c>
-      <c r="C8" t="s">
-        <v>83</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H8" t="s">
         <v>4</v>
       </c>
       <c r="J8" s="3">
         <v>43890</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
@@ -1076,22 +1166,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H9" t="s">
         <v>4</v>
@@ -1105,22 +1195,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H10" t="s">
         <v>4</v>
@@ -1134,22 +1224,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H11" t="s">
         <v>13</v>
@@ -1163,16 +1253,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F12" t="s">
         <v>6</v>
@@ -1181,7 +1271,7 @@
         <v>4</v>
       </c>
       <c r="I12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J12" s="3">
         <v>43890</v>
@@ -1193,16 +1283,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
         <v>82</v>
-      </c>
-      <c r="C13" t="s">
-        <v>83</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F13" t="s">
         <v>6</v>
@@ -1219,28 +1309,28 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H14" t="s">
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J14" s="3">
         <v>43891</v>
@@ -1251,22 +1341,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H15" t="s">
         <v>4</v>
@@ -1280,16 +1370,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
@@ -1298,7 +1388,7 @@
         <v>4</v>
       </c>
       <c r="I16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J16" s="3">
         <v>43891</v>
@@ -1309,22 +1399,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H17" t="s">
         <v>4</v>
@@ -1338,16 +1428,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" t="s">
         <v>6</v>
@@ -1364,16 +1454,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" t="s">
         <v>6</v>
@@ -1390,22 +1480,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H20" t="s">
         <v>4</v>
@@ -1419,22 +1509,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
         <v>82</v>
-      </c>
-      <c r="C21" t="s">
-        <v>83</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H21" t="s">
         <v>4</v>
@@ -1448,22 +1538,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H22" t="s">
         <v>4</v>
@@ -1477,22 +1567,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D23" t="s">
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H23" t="s">
         <v>4</v>
@@ -1506,22 +1596,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" t="s">
         <v>78</v>
       </c>
-      <c r="E24" t="s">
-        <v>79</v>
-      </c>
       <c r="F24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H24" t="s">
         <v>13</v>
@@ -1535,22 +1625,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" t="s">
         <v>78</v>
       </c>
-      <c r="E25" t="s">
-        <v>79</v>
-      </c>
       <c r="F25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G25" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H25" t="s">
         <v>4</v>
@@ -1564,22 +1654,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H26" t="s">
         <v>4</v>
@@ -1593,22 +1683,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" t="s">
         <v>82</v>
-      </c>
-      <c r="C27" t="s">
-        <v>83</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H27" t="s">
         <v>4</v>
@@ -1622,22 +1712,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H28" t="s">
         <v>4</v>
@@ -1651,22 +1741,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H29" t="s">
         <v>4</v>
@@ -1683,22 +1773,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H30" t="s">
         <v>4</v>
@@ -1715,22 +1805,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H31" t="s">
         <v>13</v>
@@ -1744,22 +1834,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
@@ -1773,10 +1863,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
         <v>82</v>
-      </c>
-      <c r="C33" t="s">
-        <v>83</v>
       </c>
       <c r="D33" t="s">
         <v>25</v>
@@ -1785,10 +1875,10 @@
         <v>26</v>
       </c>
       <c r="F33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H33" t="s">
         <v>4</v>
@@ -1802,10 +1892,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D34" t="s">
         <v>27</v>
@@ -1814,10 +1904,10 @@
         <v>28</v>
       </c>
       <c r="F34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H34" t="s">
         <v>4</v>
@@ -1831,10 +1921,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D35" t="s">
         <v>27</v>
@@ -1843,10 +1933,10 @@
         <v>28</v>
       </c>
       <c r="F35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H35" t="s">
         <v>4</v>
@@ -1860,10 +1950,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D36" t="s">
         <v>25</v>
@@ -1886,10 +1976,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D37" t="s">
         <v>27</v>
@@ -1898,10 +1988,10 @@
         <v>29</v>
       </c>
       <c r="F37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H37" t="s">
         <v>4</v>
@@ -1915,13 +2005,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" t="s">
-        <v>45</v>
+        <v>82</v>
+      </c>
+      <c r="D38" t="s">
+        <v>44</v>
       </c>
       <c r="F38" t="s">
         <v>6</v>
@@ -1938,19 +2028,19 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" t="s">
         <v>11</v>
       </c>
       <c r="F39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H39" t="s">
         <v>4</v>
@@ -1964,10 +2054,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D40" t="s">
         <v>27</v>
@@ -1976,10 +2066,10 @@
         <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H40" t="s">
         <v>13</v>
@@ -1993,10 +2083,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D41" t="s">
         <v>27</v>
@@ -2005,10 +2095,10 @@
         <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H41" t="s">
         <v>4</v>
@@ -2022,10 +2112,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D42" t="s">
         <v>27</v>
@@ -2034,10 +2124,10 @@
         <v>8</v>
       </c>
       <c r="F42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H42" t="s">
         <v>4</v>
@@ -2051,10 +2141,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D43" t="s">
         <v>27</v>
@@ -2063,10 +2153,10 @@
         <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H43" t="s">
         <v>4</v>
@@ -2080,10 +2170,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" t="s">
         <v>82</v>
-      </c>
-      <c r="C44" t="s">
-        <v>83</v>
       </c>
       <c r="D44" t="s">
         <v>30</v>
@@ -2092,7 +2182,7 @@
         <v>13</v>
       </c>
       <c r="F44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G44" t="s">
         <v>13</v>
@@ -2109,16 +2199,16 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D45" t="s">
         <v>25</v>
       </c>
       <c r="E45" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="F45" t="s">
         <v>6</v>
@@ -2135,16 +2225,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D46" t="s">
         <v>27</v>
       </c>
       <c r="E46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F46" t="s">
         <v>6</v>
@@ -2161,22 +2251,22 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D47" t="s">
         <v>27</v>
       </c>
       <c r="E47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H47" t="s">
         <v>4</v>
@@ -2190,22 +2280,22 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D48" t="s">
         <v>27</v>
       </c>
       <c r="E48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H48" t="s">
         <v>4</v>
@@ -2219,22 +2309,22 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D49" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" t="s">
         <v>35</v>
       </c>
-      <c r="E49" t="s">
-        <v>36</v>
-      </c>
       <c r="F49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H49" t="s">
         <v>4</v>
@@ -2248,22 +2338,22 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D50" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" t="s">
         <v>37</v>
       </c>
-      <c r="E50" t="s">
-        <v>38</v>
-      </c>
       <c r="F50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H50" t="s">
         <v>4</v>
@@ -2280,22 +2370,22 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D51" t="s">
         <v>27</v>
       </c>
       <c r="E51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H51" t="s">
         <v>4</v>
@@ -2309,22 +2399,22 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D52" t="s">
+        <v>39</v>
+      </c>
+      <c r="E52" t="s">
         <v>40</v>
       </c>
-      <c r="E52" t="s">
-        <v>41</v>
-      </c>
       <c r="F52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H52" t="s">
         <v>4</v>
@@ -2338,16 +2428,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D53" t="s">
         <v>27</v>
       </c>
       <c r="E53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F53" t="s">
         <v>6</v>
@@ -2364,16 +2454,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D54" t="s">
         <v>27</v>
       </c>
       <c r="E54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F54" t="s">
         <v>6</v>
@@ -2390,22 +2480,22 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D55" t="s">
         <v>27</v>
       </c>
       <c r="E55" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H55" t="s">
         <v>4</v>
@@ -2419,22 +2509,22 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D56" t="s">
         <v>27</v>
       </c>
       <c r="E56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H56" t="s">
         <v>4</v>
@@ -2448,22 +2538,22 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D57" t="s">
         <v>27</v>
       </c>
       <c r="E57" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H57" t="s">
         <v>4</v>
@@ -2477,10 +2567,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D58" t="s">
         <v>25</v>
@@ -2489,7 +2579,7 @@
         <v>13</v>
       </c>
       <c r="F58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G58" t="s">
         <v>13</v>
@@ -2506,22 +2596,22 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D59" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" t="s">
         <v>35</v>
       </c>
-      <c r="E59" t="s">
-        <v>36</v>
-      </c>
       <c r="F59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H59" t="s">
         <v>4</v>
@@ -2535,22 +2625,22 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D60" t="s">
+        <v>42</v>
+      </c>
+      <c r="E60" t="s">
         <v>43</v>
       </c>
-      <c r="E60" t="s">
-        <v>44</v>
-      </c>
       <c r="F60" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G60" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H60" t="s">
         <v>4</v>
@@ -2564,10 +2654,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D61" t="s">
         <v>5</v>
@@ -2576,7 +2666,7 @@
         <v>13</v>
       </c>
       <c r="F61" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G61" t="s">
         <v>13</v>
@@ -2593,10 +2683,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
@@ -2619,10 +2709,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C63" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
@@ -2631,10 +2721,10 @@
         <v>13</v>
       </c>
       <c r="F63" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H63" t="s">
         <v>4</v>
@@ -2648,22 +2738,22 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D64" t="s">
         <v>8</v>
       </c>
       <c r="E64" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F64" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G64" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H64" t="s">
         <v>4</v>
@@ -2677,22 +2767,22 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D65" t="s">
         <v>8</v>
       </c>
       <c r="E65" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G65" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H65" t="s">
         <v>4</v>
@@ -2706,22 +2796,22 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C66" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D66" t="s">
         <v>8</v>
       </c>
       <c r="E66" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F66" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G66" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H66" t="s">
         <v>4</v>
@@ -2735,10 +2825,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C67" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D67" t="s">
         <v>11</v>
@@ -2747,10 +2837,10 @@
         <v>13</v>
       </c>
       <c r="F67" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H67" t="s">
         <v>4</v>
@@ -2764,10 +2854,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C68" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D68" t="s">
         <v>20</v>
@@ -2790,22 +2880,22 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D69" t="s">
         <v>8</v>
       </c>
       <c r="E69" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F69" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G69" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H69" t="s">
         <v>4</v>
@@ -2819,22 +2909,22 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D70" t="s">
         <v>8</v>
       </c>
       <c r="E70" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G70" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H70" t="s">
         <v>4</v>
@@ -2848,22 +2938,22 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D71" t="s">
         <v>8</v>
       </c>
       <c r="E71" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F71" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G71" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H71" t="s">
         <v>4</v>
@@ -2877,16 +2967,16 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C72" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D72" t="s">
         <v>8</v>
       </c>
       <c r="E72" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F72" t="s">
         <v>6</v>
@@ -2903,10 +2993,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D73" t="s">
         <v>7</v>
@@ -2915,7 +3005,7 @@
         <v>13</v>
       </c>
       <c r="F73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G73" t="s">
         <v>13</v>
@@ -2932,10 +3022,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C74" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D74" t="s">
         <v>9</v>
@@ -2944,10 +3034,10 @@
         <v>13</v>
       </c>
       <c r="F74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H74" t="s">
         <v>4</v>
@@ -2964,10 +3054,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D75" t="s">
         <v>7</v>
@@ -2976,7 +3066,7 @@
         <v>13</v>
       </c>
       <c r="F75" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G75" t="s">
         <v>13</v>
@@ -3201,10 +3291,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C84" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D84" t="s">
         <v>8</v>
@@ -3253,22 +3343,22 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C86" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D86" t="s">
         <v>9</v>
       </c>
       <c r="E86" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G86" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H86" t="s">
         <v>4</v>
@@ -3308,22 +3398,22 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C88" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D88" t="s">
         <v>22</v>
       </c>
       <c r="E88" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F88" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G88" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H88" t="s">
         <v>4</v>
@@ -3441,16 +3531,16 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C93" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D93" t="s">
         <v>12</v>
       </c>
       <c r="E93" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F93" t="s">
         <v>13</v>
@@ -3467,22 +3557,22 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C94" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D94" t="s">
+        <v>49</v>
+      </c>
+      <c r="E94" t="s">
         <v>50</v>
       </c>
-      <c r="E94" t="s">
-        <v>51</v>
-      </c>
       <c r="F94" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G94" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H94" t="s">
         <v>4</v>
@@ -3548,22 +3638,22 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
+        <v>81</v>
+      </c>
+      <c r="C97" t="s">
         <v>82</v>
-      </c>
-      <c r="C97" t="s">
-        <v>83</v>
       </c>
       <c r="D97" t="s">
         <v>22</v>
       </c>
       <c r="E97" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F97" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G97" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H97" t="s">
         <v>4</v>
@@ -3577,22 +3667,22 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C98" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D98" t="s">
         <v>22</v>
       </c>
       <c r="E98" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G98" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H98" t="s">
         <v>4</v>
@@ -3612,7 +3702,7 @@
         <v>13</v>
       </c>
       <c r="D99" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E99" t="s">
         <v>13</v>
@@ -3632,22 +3722,22 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C100" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D100" t="s">
         <v>3</v>
       </c>
       <c r="E100" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F100" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G100" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H100" t="s">
         <v>4</v>
@@ -4086,7 +4176,7 @@
         <v>13</v>
       </c>
       <c r="D117" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E117" t="s">
         <v>13</v>
@@ -4132,22 +4222,22 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C119" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D119" t="s">
         <v>20</v>
       </c>
       <c r="E119" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F119" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G119" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H119" t="s">
         <v>4</v>
@@ -4944,22 +5034,22 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C150" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D150" t="s">
+        <v>56</v>
+      </c>
+      <c r="E150" t="s">
         <v>57</v>
       </c>
-      <c r="E150" t="s">
-        <v>58</v>
-      </c>
       <c r="F150" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G150" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H150" t="s">
         <v>4</v>
@@ -4973,16 +5063,16 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C151" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D151" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E151" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F151" t="s">
         <v>6</v>
@@ -5155,22 +5245,22 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C158" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D158" t="s">
         <v>3</v>
       </c>
       <c r="E158" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F158" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G158" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H158" t="s">
         <v>4</v>
@@ -5886,22 +5976,22 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C186" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D186" t="s">
         <v>5</v>
       </c>
       <c r="E186" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F186" t="s">
+        <v>120</v>
+      </c>
+      <c r="G186" t="s">
         <v>121</v>
-      </c>
-      <c r="G186" t="s">
-        <v>122</v>
       </c>
       <c r="H186" t="s">
         <v>4</v>
@@ -6019,10 +6109,10 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C191" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D191" t="s">
         <v>3</v>
@@ -6031,10 +6121,10 @@
         <v>13</v>
       </c>
       <c r="F191" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G191" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H191" t="s">
         <v>4</v>
@@ -6048,10 +6138,10 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C192" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D192" t="s">
         <v>5</v>
@@ -6074,10 +6164,10 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C193" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D193" t="s">
         <v>7</v>
@@ -6086,10 +6176,10 @@
         <v>13</v>
       </c>
       <c r="F193" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G193" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H193" t="s">
         <v>4</v>
@@ -6103,10 +6193,10 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C194" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D194" t="s">
         <v>8</v>
@@ -6115,10 +6205,10 @@
         <v>13</v>
       </c>
       <c r="F194" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G194" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H194" t="s">
         <v>4</v>
@@ -6132,10 +6222,10 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C195" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D195" t="s">
         <v>8</v>
@@ -6144,10 +6234,10 @@
         <v>13</v>
       </c>
       <c r="F195" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G195" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H195" t="s">
         <v>4</v>
@@ -6161,10 +6251,10 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C196" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D196" t="s">
         <v>3</v>
@@ -6173,10 +6263,10 @@
         <v>13</v>
       </c>
       <c r="F196" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G196" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H196" t="s">
         <v>4</v>
@@ -6190,10 +6280,10 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C197" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D197" t="s">
         <v>3</v>
@@ -6202,10 +6292,10 @@
         <v>13</v>
       </c>
       <c r="F197" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G197" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H197" t="s">
         <v>4</v>
@@ -6219,10 +6309,10 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C198" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D198" t="s">
         <v>7</v>
@@ -6245,10 +6335,10 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
+        <v>81</v>
+      </c>
+      <c r="C199" t="s">
         <v>82</v>
-      </c>
-      <c r="C199" t="s">
-        <v>83</v>
       </c>
       <c r="D199" t="s">
         <v>8</v>
@@ -6257,10 +6347,10 @@
         <v>13</v>
       </c>
       <c r="F199" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G199" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H199" t="s">
         <v>4</v>
@@ -6274,10 +6364,10 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C200" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D200" t="s">
         <v>3</v>
@@ -6300,10 +6390,10 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C201" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D201" t="s">
         <v>9</v>
@@ -6312,10 +6402,10 @@
         <v>13</v>
       </c>
       <c r="F201" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G201" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H201" t="s">
         <v>4</v>
@@ -6329,10 +6419,10 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C202" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D202" t="s">
         <v>10</v>
@@ -6341,10 +6431,10 @@
         <v>13</v>
       </c>
       <c r="F202" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G202" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H202" t="s">
         <v>4</v>
@@ -6358,10 +6448,10 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C203" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D203" t="s">
         <v>11</v>
@@ -6370,10 +6460,10 @@
         <v>13</v>
       </c>
       <c r="F203" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G203" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H203" t="s">
         <v>4</v>
@@ -6387,10 +6477,10 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C204" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D204" t="s">
         <v>12</v>
@@ -6413,10 +6503,10 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C205" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D205" t="s">
         <v>10</v>
@@ -6425,10 +6515,10 @@
         <v>13</v>
       </c>
       <c r="F205" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G205" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H205" t="s">
         <v>4</v>
@@ -6442,10 +6532,10 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
+        <v>81</v>
+      </c>
+      <c r="C206" t="s">
         <v>82</v>
-      </c>
-      <c r="C206" t="s">
-        <v>83</v>
       </c>
       <c r="D206" t="s">
         <v>14</v>
@@ -6454,10 +6544,10 @@
         <v>13</v>
       </c>
       <c r="F206" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G206" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H206" t="s">
         <v>4</v>
@@ -6471,10 +6561,10 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C207" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D207" t="s">
         <v>15</v>
@@ -6483,10 +6573,10 @@
         <v>13</v>
       </c>
       <c r="F207" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G207" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H207" t="s">
         <v>4</v>
@@ -6500,10 +6590,10 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C208" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D208" t="s">
         <v>16</v>
@@ -6512,10 +6602,10 @@
         <v>13</v>
       </c>
       <c r="F208" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G208" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H208" t="s">
         <v>4</v>
@@ -6529,10 +6619,10 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C209" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D209" t="s">
         <v>17</v>
@@ -6541,10 +6631,10 @@
         <v>13</v>
       </c>
       <c r="F209" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G209" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H209" t="s">
         <v>4</v>
@@ -6558,10 +6648,10 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C210" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D210" t="s">
         <v>18</v>
@@ -6570,10 +6660,10 @@
         <v>13</v>
       </c>
       <c r="F210" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G210" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H210" t="s">
         <v>4</v>
@@ -6665,10 +6755,10 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
+        <v>81</v>
+      </c>
+      <c r="C214" t="s">
         <v>82</v>
-      </c>
-      <c r="C214" t="s">
-        <v>83</v>
       </c>
       <c r="D214" t="s">
         <v>20</v>
@@ -6677,7 +6767,7 @@
         <v>13</v>
       </c>
       <c r="F214" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G214" t="s">
         <v>13</v>
@@ -6694,10 +6784,10 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C215" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D215" t="s">
         <v>14</v>
@@ -6706,10 +6796,10 @@
         <v>13</v>
       </c>
       <c r="F215" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G215" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H215" t="s">
         <v>4</v>
@@ -6723,10 +6813,10 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C216" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D216" t="s">
         <v>11</v>
@@ -6735,10 +6825,10 @@
         <v>13</v>
       </c>
       <c r="F216" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G216" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H216" t="s">
         <v>4</v>
@@ -6747,15 +6837,15 @@
         <v>43908</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C217" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D217" t="s">
         <v>11</v>
@@ -6764,10 +6854,10 @@
         <v>13</v>
       </c>
       <c r="F217" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G217" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H217" t="s">
         <v>4</v>
@@ -6776,15 +6866,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C218" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D218" t="s">
         <v>21</v>
@@ -6793,10 +6883,10 @@
         <v>13</v>
       </c>
       <c r="F218" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G218" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H218" t="s">
         <v>4</v>
@@ -6805,15 +6895,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C219" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D219" t="s">
         <v>3</v>
@@ -6822,10 +6912,10 @@
         <v>13</v>
       </c>
       <c r="F219" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G219" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H219" t="s">
         <v>4</v>
@@ -6834,15 +6924,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>219</v>
       </c>
       <c r="B220" t="s">
+        <v>81</v>
+      </c>
+      <c r="C220" t="s">
         <v>82</v>
-      </c>
-      <c r="C220" t="s">
-        <v>83</v>
       </c>
       <c r="D220" t="s">
         <v>3</v>
@@ -6851,10 +6941,10 @@
         <v>13</v>
       </c>
       <c r="F220" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G220" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H220" t="s">
         <v>4</v>
@@ -6863,15 +6953,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C221" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D221" t="s">
         <v>7</v>
@@ -6880,10 +6970,10 @@
         <v>13</v>
       </c>
       <c r="F221" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G221" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H221" t="s">
         <v>13</v>
@@ -6892,15 +6982,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C222" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D222" t="s">
         <v>10</v>
@@ -6909,10 +6999,10 @@
         <v>13</v>
       </c>
       <c r="F222" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G222" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H222" t="s">
         <v>4</v>
@@ -6921,15 +7011,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C223" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D223" t="s">
         <v>8</v>
@@ -6938,10 +7028,10 @@
         <v>13</v>
       </c>
       <c r="F223" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G223" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H223" t="s">
         <v>4</v>
@@ -6950,15 +7040,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C224" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D224" t="s">
         <v>10</v>
@@ -6967,10 +7057,10 @@
         <v>13</v>
       </c>
       <c r="F224" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G224" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H224" t="s">
         <v>4</v>
@@ -6979,15 +7069,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C225" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D225" t="s">
         <v>8</v>
@@ -7005,15 +7095,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C226" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D226" t="s">
         <v>9</v>
@@ -7031,15 +7121,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C227" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D227" t="s">
         <v>8</v>
@@ -7057,15 +7147,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C228" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D228" t="s">
         <v>8</v>
@@ -7083,15 +7173,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C229" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D229" t="s">
         <v>8</v>
@@ -7109,15 +7199,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C230" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D230" t="s">
         <v>8</v>
@@ -7135,15 +7225,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C231" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D231" t="s">
         <v>22</v>
@@ -7161,15 +7251,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C232" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D232" t="s">
         <v>8</v>
@@ -7187,15 +7277,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C233" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D233" t="s">
         <v>8</v>
@@ -7213,15 +7303,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C234" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D234" t="s">
         <v>7</v>
@@ -7230,10 +7320,10 @@
         <v>13</v>
       </c>
       <c r="F234" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G234" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H234" t="s">
         <v>4</v>
@@ -7242,15 +7332,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C235" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D235" t="s">
         <v>7</v>
@@ -7259,10 +7349,10 @@
         <v>13</v>
       </c>
       <c r="F235" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G235" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H235" t="s">
         <v>13</v>
@@ -7271,15 +7361,15 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C236" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D236" t="s">
         <v>24</v>
@@ -7288,10 +7378,10 @@
         <v>13</v>
       </c>
       <c r="F236" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G236" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H236" t="s">
         <v>13</v>
@@ -7300,7 +7390,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>236</v>
       </c>
@@ -7326,7 +7416,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>237</v>
       </c>
@@ -7352,7 +7442,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>238</v>
       </c>
@@ -7378,7 +7468,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>239</v>
       </c>
@@ -7404,7 +7494,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>240</v>
       </c>
@@ -7430,7 +7520,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>241</v>
       </c>
@@ -7456,7 +7546,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>242</v>
       </c>
@@ -7482,7 +7572,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>243</v>
       </c>
@@ -7508,7 +7598,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>244</v>
       </c>
@@ -7534,7 +7624,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>245</v>
       </c>
@@ -7560,7 +7650,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>246</v>
       </c>
@@ -7586,7 +7676,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>247</v>
       </c>
@@ -7612,7 +7702,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>248</v>
       </c>
@@ -7638,7 +7728,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>249</v>
       </c>
@@ -7664,7 +7754,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>250</v>
       </c>
@@ -7690,7 +7780,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>251</v>
       </c>
@@ -7716,7 +7806,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>252</v>
       </c>
@@ -7742,7 +7832,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>252</v>
       </c>
@@ -7768,7 +7858,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>254</v>
       </c>
@@ -7794,7 +7884,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>255</v>
       </c>
@@ -7820,7 +7910,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>256</v>
       </c>
@@ -7846,7 +7936,7 @@
         <v>43909</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A258">
         <v>257</v>
       </c>
@@ -7872,10 +7962,1140 @@
         <v>43909</v>
       </c>
     </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A259">
+        <v>258</v>
+      </c>
+      <c r="B259" t="s">
+        <v>81</v>
+      </c>
+      <c r="C259" t="s">
+        <v>82</v>
+      </c>
+      <c r="D259" t="s">
+        <v>3</v>
+      </c>
+      <c r="E259" t="s">
+        <v>19</v>
+      </c>
+      <c r="F259" t="s">
+        <v>19</v>
+      </c>
+      <c r="H259" t="s">
+        <v>145</v>
+      </c>
+      <c r="J259" s="3">
+        <v>43908</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A260">
+        <v>259</v>
+      </c>
+      <c r="B260" t="s">
+        <v>88</v>
+      </c>
+      <c r="C260" t="s">
+        <v>82</v>
+      </c>
+      <c r="D260" t="s">
+        <v>10</v>
+      </c>
+      <c r="F260" t="s">
+        <v>146</v>
+      </c>
+      <c r="H260" t="s">
+        <v>4</v>
+      </c>
+      <c r="J260" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A261">
+        <v>260</v>
+      </c>
+      <c r="B261" t="s">
+        <v>87</v>
+      </c>
+      <c r="C261" t="s">
+        <v>82</v>
+      </c>
+      <c r="D261" t="s">
+        <v>147</v>
+      </c>
+      <c r="F261" t="s">
+        <v>6</v>
+      </c>
+      <c r="H261" t="s">
+        <v>4</v>
+      </c>
+      <c r="J261" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A262">
+        <v>261</v>
+      </c>
+      <c r="B262" t="s">
+        <v>85</v>
+      </c>
+      <c r="C262" t="s">
+        <v>83</v>
+      </c>
+      <c r="D262" t="s">
+        <v>147</v>
+      </c>
+      <c r="F262" t="s">
+        <v>148</v>
+      </c>
+      <c r="H262" t="s">
+        <v>4</v>
+      </c>
+      <c r="J262" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A263">
+        <v>262</v>
+      </c>
+      <c r="B263" t="s">
+        <v>85</v>
+      </c>
+      <c r="C263" t="s">
+        <v>82</v>
+      </c>
+      <c r="D263" t="s">
+        <v>147</v>
+      </c>
+      <c r="F263" t="s">
+        <v>148</v>
+      </c>
+      <c r="H263" t="s">
+        <v>4</v>
+      </c>
+      <c r="J263" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A264">
+        <v>263</v>
+      </c>
+      <c r="B264" t="s">
+        <v>89</v>
+      </c>
+      <c r="C264" t="s">
+        <v>83</v>
+      </c>
+      <c r="D264" t="s">
+        <v>22</v>
+      </c>
+      <c r="F264" t="s">
+        <v>149</v>
+      </c>
+      <c r="H264" t="s">
+        <v>4</v>
+      </c>
+      <c r="J264" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A265">
+        <v>264</v>
+      </c>
+      <c r="B265" t="s">
+        <v>86</v>
+      </c>
+      <c r="C265" t="s">
+        <v>82</v>
+      </c>
+      <c r="D265" t="s">
+        <v>150</v>
+      </c>
+      <c r="F265" t="s">
+        <v>151</v>
+      </c>
+      <c r="H265" t="s">
+        <v>4</v>
+      </c>
+      <c r="J265" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A266">
+        <v>265</v>
+      </c>
+      <c r="B266" t="s">
+        <v>85</v>
+      </c>
+      <c r="C266" t="s">
+        <v>82</v>
+      </c>
+      <c r="D266" t="s">
+        <v>22</v>
+      </c>
+      <c r="F266" t="s">
+        <v>13</v>
+      </c>
+      <c r="H266" t="s">
+        <v>152</v>
+      </c>
+      <c r="J266" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A267">
+        <v>266</v>
+      </c>
+      <c r="B267" t="s">
+        <v>155</v>
+      </c>
+      <c r="C267" t="s">
+        <v>83</v>
+      </c>
+      <c r="D267" t="s">
+        <v>22</v>
+      </c>
+      <c r="F267" t="s">
+        <v>13</v>
+      </c>
+      <c r="H267" t="s">
+        <v>152</v>
+      </c>
+      <c r="J267" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A268">
+        <v>267</v>
+      </c>
+      <c r="B268" t="s">
+        <v>86</v>
+      </c>
+      <c r="C268" t="s">
+        <v>83</v>
+      </c>
+      <c r="D268" t="s">
+        <v>22</v>
+      </c>
+      <c r="F268" t="s">
+        <v>13</v>
+      </c>
+      <c r="H268" t="s">
+        <v>152</v>
+      </c>
+      <c r="J268" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A269">
+        <v>268</v>
+      </c>
+      <c r="B269" t="s">
+        <v>89</v>
+      </c>
+      <c r="C269" t="s">
+        <v>82</v>
+      </c>
+      <c r="D269" t="s">
+        <v>22</v>
+      </c>
+      <c r="F269" t="s">
+        <v>13</v>
+      </c>
+      <c r="H269" t="s">
+        <v>152</v>
+      </c>
+      <c r="J269" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A270">
+        <v>269</v>
+      </c>
+      <c r="B270" t="s">
+        <v>86</v>
+      </c>
+      <c r="C270" t="s">
+        <v>82</v>
+      </c>
+      <c r="D270" t="s">
+        <v>11</v>
+      </c>
+      <c r="F270" t="s">
+        <v>153</v>
+      </c>
+      <c r="H270" t="s">
+        <v>4</v>
+      </c>
+      <c r="J270" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A271">
+        <v>270</v>
+      </c>
+      <c r="B271" t="s">
+        <v>88</v>
+      </c>
+      <c r="C271" t="s">
+        <v>82</v>
+      </c>
+      <c r="D271" t="s">
+        <v>11</v>
+      </c>
+      <c r="F271" t="s">
+        <v>6</v>
+      </c>
+      <c r="H271" t="s">
+        <v>4</v>
+      </c>
+      <c r="J271" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A272">
+        <v>271</v>
+      </c>
+      <c r="B272" t="s">
+        <v>88</v>
+      </c>
+      <c r="C272" t="s">
+        <v>82</v>
+      </c>
+      <c r="D272" t="s">
+        <v>11</v>
+      </c>
+      <c r="F272" t="s">
+        <v>6</v>
+      </c>
+      <c r="H272" t="s">
+        <v>4</v>
+      </c>
+      <c r="J272" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A273">
+        <v>272</v>
+      </c>
+      <c r="B273" t="s">
+        <v>89</v>
+      </c>
+      <c r="C273" t="s">
+        <v>83</v>
+      </c>
+      <c r="D273" t="s">
+        <v>10</v>
+      </c>
+      <c r="F273" t="s">
+        <v>149</v>
+      </c>
+      <c r="H273" t="s">
+        <v>4</v>
+      </c>
+      <c r="J273" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="274" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A274">
+        <v>273</v>
+      </c>
+      <c r="B274" t="s">
+        <v>89</v>
+      </c>
+      <c r="C274" t="s">
+        <v>82</v>
+      </c>
+      <c r="D274" t="s">
+        <v>9</v>
+      </c>
+      <c r="F274" t="s">
+        <v>13</v>
+      </c>
+      <c r="H274" t="s">
+        <v>23</v>
+      </c>
+      <c r="J274" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A275">
+        <v>274</v>
+      </c>
+      <c r="B275" t="s">
+        <v>84</v>
+      </c>
+      <c r="C275" t="s">
+        <v>83</v>
+      </c>
+      <c r="D275" t="s">
+        <v>7</v>
+      </c>
+      <c r="F275" t="s">
+        <v>6</v>
+      </c>
+      <c r="H275" t="s">
+        <v>4</v>
+      </c>
+      <c r="J275" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="276" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A276">
+        <v>275</v>
+      </c>
+      <c r="B276" t="s">
+        <v>88</v>
+      </c>
+      <c r="C276" t="s">
+        <v>83</v>
+      </c>
+      <c r="D276" t="s">
+        <v>8</v>
+      </c>
+      <c r="F276" t="s">
+        <v>6</v>
+      </c>
+      <c r="H276" t="s">
+        <v>4</v>
+      </c>
+      <c r="J276" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A277">
+        <v>276</v>
+      </c>
+      <c r="B277" t="s">
+        <v>88</v>
+      </c>
+      <c r="C277" t="s">
+        <v>82</v>
+      </c>
+      <c r="D277" t="s">
+        <v>7</v>
+      </c>
+      <c r="F277" t="s">
+        <v>13</v>
+      </c>
+      <c r="H277" t="s">
+        <v>4</v>
+      </c>
+      <c r="J277" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A278">
+        <v>277</v>
+      </c>
+      <c r="B278" t="s">
+        <v>84</v>
+      </c>
+      <c r="C278" t="s">
+        <v>83</v>
+      </c>
+      <c r="D278" t="s">
+        <v>9</v>
+      </c>
+      <c r="F278" t="s">
+        <v>6</v>
+      </c>
+      <c r="H278" t="s">
+        <v>4</v>
+      </c>
+      <c r="J278" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A279">
+        <v>278</v>
+      </c>
+      <c r="B279" t="s">
+        <v>81</v>
+      </c>
+      <c r="C279" t="s">
+        <v>83</v>
+      </c>
+      <c r="D279" t="s">
+        <v>9</v>
+      </c>
+      <c r="F279" t="s">
+        <v>149</v>
+      </c>
+      <c r="H279" t="s">
+        <v>4</v>
+      </c>
+      <c r="J279" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A280">
+        <v>279</v>
+      </c>
+      <c r="B280" t="s">
+        <v>84</v>
+      </c>
+      <c r="C280" t="s">
+        <v>82</v>
+      </c>
+      <c r="D280" t="s">
+        <v>9</v>
+      </c>
+      <c r="F280" t="s">
+        <v>6</v>
+      </c>
+      <c r="H280" t="s">
+        <v>4</v>
+      </c>
+      <c r="J280" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A281">
+        <v>280</v>
+      </c>
+      <c r="B281" t="s">
+        <v>81</v>
+      </c>
+      <c r="C281" t="s">
+        <v>83</v>
+      </c>
+      <c r="D281" t="s">
+        <v>8</v>
+      </c>
+      <c r="F281" t="s">
+        <v>6</v>
+      </c>
+      <c r="H281" t="s">
+        <v>4</v>
+      </c>
+      <c r="J281" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A282">
+        <v>281</v>
+      </c>
+      <c r="B282" t="s">
+        <v>81</v>
+      </c>
+      <c r="C282" t="s">
+        <v>83</v>
+      </c>
+      <c r="D282" t="s">
+        <v>22</v>
+      </c>
+      <c r="F282" t="s">
+        <v>6</v>
+      </c>
+      <c r="H282" t="s">
+        <v>23</v>
+      </c>
+      <c r="J282" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A283">
+        <v>282</v>
+      </c>
+      <c r="B283" t="s">
+        <v>87</v>
+      </c>
+      <c r="C283" t="s">
+        <v>82</v>
+      </c>
+      <c r="D283" t="s">
+        <v>5</v>
+      </c>
+      <c r="F283" t="s">
+        <v>154</v>
+      </c>
+      <c r="H283" t="s">
+        <v>4</v>
+      </c>
+      <c r="J283" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A284">
+        <v>283</v>
+      </c>
+      <c r="B284" t="s">
+        <v>13</v>
+      </c>
+      <c r="D284" t="s">
+        <v>13</v>
+      </c>
+      <c r="F284" t="s">
+        <v>13</v>
+      </c>
+      <c r="H284" t="s">
+        <v>13</v>
+      </c>
+      <c r="J284" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A285">
+        <v>284</v>
+      </c>
+      <c r="B285" t="s">
+        <v>13</v>
+      </c>
+      <c r="D285" t="s">
+        <v>13</v>
+      </c>
+      <c r="F285" t="s">
+        <v>19</v>
+      </c>
+      <c r="H285" t="s">
+        <v>13</v>
+      </c>
+      <c r="J285" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A286">
+        <v>285</v>
+      </c>
+      <c r="B286" t="s">
+        <v>13</v>
+      </c>
+      <c r="D286" t="s">
+        <v>13</v>
+      </c>
+      <c r="F286" t="s">
+        <v>19</v>
+      </c>
+      <c r="H286" t="s">
+        <v>13</v>
+      </c>
+      <c r="J286" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A287">
+        <v>286</v>
+      </c>
+      <c r="B287" t="s">
+        <v>13</v>
+      </c>
+      <c r="D287" t="s">
+        <v>13</v>
+      </c>
+      <c r="F287" t="s">
+        <v>13</v>
+      </c>
+      <c r="H287" t="s">
+        <v>13</v>
+      </c>
+      <c r="J287" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A288">
+        <v>287</v>
+      </c>
+      <c r="B288" t="s">
+        <v>13</v>
+      </c>
+      <c r="D288" t="s">
+        <v>13</v>
+      </c>
+      <c r="F288" t="s">
+        <v>19</v>
+      </c>
+      <c r="H288" t="s">
+        <v>13</v>
+      </c>
+      <c r="J288" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A289">
+        <v>288</v>
+      </c>
+      <c r="B289" t="s">
+        <v>13</v>
+      </c>
+      <c r="D289" t="s">
+        <v>13</v>
+      </c>
+      <c r="F289" t="s">
+        <v>19</v>
+      </c>
+      <c r="H289" t="s">
+        <v>13</v>
+      </c>
+      <c r="J289" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A290">
+        <v>289</v>
+      </c>
+      <c r="B290" t="s">
+        <v>13</v>
+      </c>
+      <c r="D290" t="s">
+        <v>13</v>
+      </c>
+      <c r="F290" t="s">
+        <v>13</v>
+      </c>
+      <c r="H290" t="s">
+        <v>13</v>
+      </c>
+      <c r="J290" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A291">
+        <v>290</v>
+      </c>
+      <c r="B291" t="s">
+        <v>13</v>
+      </c>
+      <c r="D291" t="s">
+        <v>13</v>
+      </c>
+      <c r="F291" t="s">
+        <v>19</v>
+      </c>
+      <c r="H291" t="s">
+        <v>13</v>
+      </c>
+      <c r="J291" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A292">
+        <v>291</v>
+      </c>
+      <c r="B292" t="s">
+        <v>13</v>
+      </c>
+      <c r="D292" t="s">
+        <v>13</v>
+      </c>
+      <c r="F292" t="s">
+        <v>19</v>
+      </c>
+      <c r="H292" t="s">
+        <v>13</v>
+      </c>
+      <c r="J292" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A293">
+        <v>292</v>
+      </c>
+      <c r="B293" t="s">
+        <v>13</v>
+      </c>
+      <c r="D293" t="s">
+        <v>13</v>
+      </c>
+      <c r="F293" t="s">
+        <v>13</v>
+      </c>
+      <c r="H293" t="s">
+        <v>13</v>
+      </c>
+      <c r="J293" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A294">
+        <v>293</v>
+      </c>
+      <c r="B294" t="s">
+        <v>13</v>
+      </c>
+      <c r="D294" t="s">
+        <v>13</v>
+      </c>
+      <c r="F294" t="s">
+        <v>19</v>
+      </c>
+      <c r="H294" t="s">
+        <v>13</v>
+      </c>
+      <c r="J294" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A295">
+        <v>294</v>
+      </c>
+      <c r="B295" t="s">
+        <v>13</v>
+      </c>
+      <c r="D295" t="s">
+        <v>13</v>
+      </c>
+      <c r="F295" t="s">
+        <v>13</v>
+      </c>
+      <c r="H295" t="s">
+        <v>13</v>
+      </c>
+      <c r="J295" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A296">
+        <v>295</v>
+      </c>
+      <c r="B296" t="s">
+        <v>13</v>
+      </c>
+      <c r="D296" t="s">
+        <v>13</v>
+      </c>
+      <c r="F296" t="s">
+        <v>19</v>
+      </c>
+      <c r="H296" t="s">
+        <v>13</v>
+      </c>
+      <c r="J296" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A297">
+        <v>296</v>
+      </c>
+      <c r="B297" t="s">
+        <v>13</v>
+      </c>
+      <c r="D297" t="s">
+        <v>13</v>
+      </c>
+      <c r="F297" t="s">
+        <v>19</v>
+      </c>
+      <c r="H297" t="s">
+        <v>13</v>
+      </c>
+      <c r="J297" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A298">
+        <v>297</v>
+      </c>
+      <c r="B298" t="s">
+        <v>13</v>
+      </c>
+      <c r="D298" t="s">
+        <v>13</v>
+      </c>
+      <c r="F298" t="s">
+        <v>13</v>
+      </c>
+      <c r="H298" t="s">
+        <v>13</v>
+      </c>
+      <c r="J298" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A299">
+        <v>298</v>
+      </c>
+      <c r="B299" t="s">
+        <v>13</v>
+      </c>
+      <c r="D299" t="s">
+        <v>13</v>
+      </c>
+      <c r="F299" t="s">
+        <v>19</v>
+      </c>
+      <c r="H299" t="s">
+        <v>13</v>
+      </c>
+      <c r="J299" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A300">
+        <v>299</v>
+      </c>
+      <c r="B300" t="s">
+        <v>13</v>
+      </c>
+      <c r="D300" t="s">
+        <v>13</v>
+      </c>
+      <c r="F300" t="s">
+        <v>19</v>
+      </c>
+      <c r="H300" t="s">
+        <v>13</v>
+      </c>
+      <c r="J300" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A301">
+        <v>300</v>
+      </c>
+      <c r="B301" t="s">
+        <v>13</v>
+      </c>
+      <c r="D301" t="s">
+        <v>13</v>
+      </c>
+      <c r="F301" t="s">
+        <v>13</v>
+      </c>
+      <c r="H301" t="s">
+        <v>13</v>
+      </c>
+      <c r="J301" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A302">
+        <v>301</v>
+      </c>
+      <c r="B302" t="s">
+        <v>13</v>
+      </c>
+      <c r="D302" t="s">
+        <v>13</v>
+      </c>
+      <c r="F302" t="s">
+        <v>19</v>
+      </c>
+      <c r="H302" t="s">
+        <v>13</v>
+      </c>
+      <c r="J302" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A303">
+        <v>302</v>
+      </c>
+      <c r="B303" t="s">
+        <v>13</v>
+      </c>
+      <c r="D303" t="s">
+        <v>13</v>
+      </c>
+      <c r="F303" t="s">
+        <v>19</v>
+      </c>
+      <c r="H303" t="s">
+        <v>13</v>
+      </c>
+      <c r="J303" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A304">
+        <v>303</v>
+      </c>
+      <c r="B304" t="s">
+        <v>13</v>
+      </c>
+      <c r="D304" t="s">
+        <v>13</v>
+      </c>
+      <c r="F304" t="s">
+        <v>19</v>
+      </c>
+      <c r="H304" t="s">
+        <v>13</v>
+      </c>
+      <c r="J304" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A305">
+        <v>304</v>
+      </c>
+      <c r="B305" t="s">
+        <v>13</v>
+      </c>
+      <c r="D305" t="s">
+        <v>13</v>
+      </c>
+      <c r="F305" t="s">
+        <v>13</v>
+      </c>
+      <c r="H305" t="s">
+        <v>13</v>
+      </c>
+      <c r="J305" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A306">
+        <v>305</v>
+      </c>
+      <c r="B306" t="s">
+        <v>13</v>
+      </c>
+      <c r="D306" t="s">
+        <v>13</v>
+      </c>
+      <c r="F306" t="s">
+        <v>19</v>
+      </c>
+      <c r="H306" t="s">
+        <v>13</v>
+      </c>
+      <c r="J306" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A307">
+        <v>306</v>
+      </c>
+      <c r="B307" t="s">
+        <v>13</v>
+      </c>
+      <c r="D307" t="s">
+        <v>13</v>
+      </c>
+      <c r="F307" t="s">
+        <v>19</v>
+      </c>
+      <c r="H307" t="s">
+        <v>13</v>
+      </c>
+      <c r="J307" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A308">
+        <v>307</v>
+      </c>
+      <c r="B308" t="s">
+        <v>13</v>
+      </c>
+      <c r="D308" t="s">
+        <v>13</v>
+      </c>
+      <c r="F308" t="s">
+        <v>13</v>
+      </c>
+      <c r="H308" t="s">
+        <v>13</v>
+      </c>
+      <c r="J308" s="3">
+        <v>43909</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A309">
+        <v>308</v>
+      </c>
+      <c r="B309" t="s">
+        <v>13</v>
+      </c>
+      <c r="D309" t="s">
+        <v>13</v>
+      </c>
+      <c r="F309" t="s">
+        <v>19</v>
+      </c>
+      <c r="H309" t="s">
+        <v>13</v>
+      </c>
+      <c r="J309" s="3">
+        <v>43909</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:R258" xr:uid="{A1FF6A91-769A-43DE-BB93-97ACEE72C0B1}"/>
+  <autoFilter ref="A1:R259" xr:uid="{A1FF6A91-769A-43DE-BB93-97ACEE72C0B1}">
+    <filterColumn colId="9">
+      <filters blank="1">
+        <dateGroupItem year="2020" month="1" dateTimeGrouping="month"/>
+        <dateGroupItem year="2020" month="2" dateTimeGrouping="month"/>
+        <dateGroupItem year="2020" month="3" day="1" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="2" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="3" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="5" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="6" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="8" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="9" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="10" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="11" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="12" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="13" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="14" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="15" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="16" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="17" dateTimeGrouping="day"/>
+        <dateGroupItem year="2020" month="3" day="18" dateTimeGrouping="day"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="L3" r:id="rId1" xr:uid="{A7060C61-A14B-4248-A10B-DC31FC64D8F2}"/>
+    <hyperlink ref="L4" r:id="rId2" xr:uid="{3C33688C-F224-49B1-B38C-F76579F73840}"/>
+    <hyperlink ref="L5" r:id="rId3" xr:uid="{E32B5FC0-8454-4818-B77F-06ECB2293A1C}"/>
+    <hyperlink ref="L6" r:id="rId4" xr:uid="{5CC6D428-1C7D-4AD9-A268-098F1BE9E240}"/>
+    <hyperlink ref="L7" r:id="rId5" xr:uid="{FDF5EF5D-256D-41E4-88D1-14F3FEB614E5}"/>
+    <hyperlink ref="L8" r:id="rId6" xr:uid="{0ADADED5-ABC1-45EE-BE35-D6F8FE8CA2D6}"/>
+    <hyperlink ref="L2" r:id="rId7" xr:uid="{9FB3C2F1-5373-4F37-ACE1-671C00F75C5A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000Internal</oddFooter>
   </headerFooter>

</xml_diff>